<commit_message>
fix car component clear
Signed-off-by: AlbertSamuelMelo <asm.asm.albert@icloud.com>
</commit_message>
<xml_diff>
--- a/API/Registers.xlsx
+++ b/API/Registers.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Registro</t>
   </si>
@@ -46,61 +46,76 @@
     <t>Hora da Validação</t>
   </si>
   <si>
-    <t>CC_1606882551310</t>
-  </si>
-  <si>
-    <t>Obra_008</t>
-  </si>
-  <si>
-    <t>NAN-4224X</t>
-  </si>
-  <si>
-    <t>MIST. (AR./BR.)</t>
-  </si>
-  <si>
-    <t>843</t>
+    <t>CC_1609634842040</t>
+  </si>
+  <si>
+    <t>Obra_067</t>
+  </si>
+  <si>
+    <t>PHA-4543</t>
+  </si>
+  <si>
+    <t>PÓ DE PEDRA</t>
+  </si>
+  <si>
+    <t>806</t>
   </si>
   <si>
     <t>null</t>
   </si>
   <si>
-    <t>-7.0587574713967</t>
-  </si>
-  <si>
-    <t>-34.8437294874933</t>
-  </si>
-  <si>
-    <t>2-12-2020</t>
-  </si>
-  <si>
-    <t>1:15</t>
+    <t>-3.07019980852851</t>
+  </si>
+  <si>
+    <t>-60.0083330533303</t>
+  </si>
+  <si>
+    <t>2-1-2021</t>
+  </si>
+  <si>
+    <t>20:47</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>CC_1606919149026</t>
-  </si>
-  <si>
-    <t>Obra_010</t>
-  </si>
-  <si>
-    <t>JXL-1146</t>
-  </si>
-  <si>
-    <t>CIMENTOS</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>-7.05866639590049</t>
-  </si>
-  <si>
-    <t>-34.8436928941033</t>
-  </si>
-  <si>
-    <t>11:25</t>
+    <t>CC_1609634868885</t>
+  </si>
+  <si>
+    <t>CC-11 A</t>
+  </si>
+  <si>
+    <t>CONCRETO</t>
+  </si>
+  <si>
+    <t>465</t>
+  </si>
+  <si>
+    <t>CC_1609634981898</t>
+  </si>
+  <si>
+    <t>NOZ-1549 N</t>
+  </si>
+  <si>
+    <t>BRITA CONTAMINADA</t>
+  </si>
+  <si>
+    <t>943</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>-3.07021826877877</t>
+  </si>
+  <si>
+    <t>-60.0083191729802</t>
+  </si>
+  <si>
+    <t>20:49</t>
+  </si>
+  <si>
+    <t>20:51</t>
   </si>
 </sst>
 </file>
@@ -481,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -568,34 +583,69 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added users to registers
Signed-off-by: AlbertSamuelMelo <asm.asm.albert@icloud.com>
</commit_message>
<xml_diff>
--- a/API/Registers.xlsx
+++ b/API/Registers.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Registro</t>
   </si>
@@ -46,67 +46,46 @@
     <t>Hora da Validação</t>
   </si>
   <si>
-    <t>CC_1609766383120</t>
-  </si>
-  <si>
-    <t>Obra_532</t>
-  </si>
-  <si>
-    <t>CC-11 A</t>
-  </si>
-  <si>
-    <t>AREIA GROSSA</t>
-  </si>
-  <si>
-    <t>764</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>-3.07019771426739</t>
-  </si>
-  <si>
-    <t>-60.0082801382892</t>
-  </si>
-  <si>
-    <t>4-1-2021</t>
-  </si>
-  <si>
-    <t>9:19</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CC_1609807972697</t>
-  </si>
-  <si>
-    <t>Obra_465</t>
-  </si>
-  <si>
-    <t>NOZ-1479</t>
-  </si>
-  <si>
-    <t>CIMENTOS</t>
-  </si>
-  <si>
-    <t>795</t>
-  </si>
-  <si>
-    <t>497</t>
-  </si>
-  <si>
-    <t>-3.07021926446465</t>
-  </si>
-  <si>
-    <t>-60.0082327702448</t>
-  </si>
-  <si>
-    <t>20:52</t>
-  </si>
-  <si>
-    <t>20:54</t>
+    <t>Criador do Registro</t>
+  </si>
+  <si>
+    <t>Validador do Registro</t>
+  </si>
+  <si>
+    <t>CC_1609929113625</t>
+  </si>
+  <si>
+    <t>Obra_001</t>
+  </si>
+  <si>
+    <t>OAK-4403</t>
+  </si>
+  <si>
+    <t>BRITA 1</t>
+  </si>
+  <si>
+    <t>341</t>
+  </si>
+  <si>
+    <t>841</t>
+  </si>
+  <si>
+    <t>-3.07022208392808</t>
+  </si>
+  <si>
+    <t>-60.0082966808251</t>
+  </si>
+  <si>
+    <t>6-1-2021</t>
+  </si>
+  <si>
+    <t>6:31</t>
+  </si>
+  <si>
+    <t>6:32</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -487,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -496,10 +475,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="11" width="20" customWidth="1"/>
+    <col min="1" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,75 +513,52 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
+      <c r="M2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>